<commit_message>
complete PIM Functinal form
</commit_message>
<xml_diff>
--- a/literature/review/potential_comparisons.xlsx
+++ b/literature/review/potential_comparisons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\School\FFparamOpt\literature\review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-workfile\PA\FFparamOpt\literature\review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7012C9-D4C4-4E7B-856E-DCA003157943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D163C7F0-F96D-4A10-B98A-5B64F6C29C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -267,11 +267,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -283,7 +283,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -292,7 +292,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -487,26 +487,68 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -520,58 +562,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4159,9 +4159,9 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4053674" cy="197875"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="4009751" cy="197875"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -4175,8 +4175,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4565650" y="10471150"/>
-              <a:ext cx="4053674" cy="197875"/>
+              <a:off x="4570046" y="10013462"/>
+              <a:ext cx="4009751" cy="197875"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4220,10 +4220,13 @@
                       </m:sSupPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑈</m:t>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" altLang="zh-CN" sz="1200" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>V</m:t>
                         </m:r>
                       </m:e>
                       <m:sup>
@@ -4251,10 +4254,10 @@
                       </m:sSupPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑈</m:t>
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑉</m:t>
                         </m:r>
                       </m:e>
                       <m:sup>
@@ -4282,10 +4285,10 @@
                       </m:sSupPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑈</m:t>
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑉</m:t>
                         </m:r>
                       </m:e>
                       <m:sup>
@@ -4313,10 +4316,10 @@
                       </m:sSupPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑈</m:t>
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑉</m:t>
                         </m:r>
                       </m:e>
                       <m:sup>
@@ -4344,10 +4347,10 @@
                       </m:sSupPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑈</m:t>
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑉</m:t>
                         </m:r>
                       </m:e>
                       <m:sup>
@@ -4373,7 +4376,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -4387,8 +4390,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4565650" y="10471150"/>
-              <a:ext cx="4053674" cy="197875"/>
+              <a:off x="4570046" y="10013462"/>
+              <a:ext cx="4009751" cy="197875"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4415,65 +4418,60 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1200" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>V^</a:t>
+              </a:r>
               <a:r>
                 <a:rPr lang="es-ES" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑈</a:t>
+                <a:t>𝑡𝑜𝑡𝑎𝑙= </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>^</a:t>
+                <a:t>𝑉^</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="es-ES" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑡𝑜𝑡𝑎𝑙= 𝑈</a:t>
+                <a:t>𝑐ℎ𝑎𝑟𝑔𝑒+ </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>^</a:t>
+                <a:t>𝑉^</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="es-ES" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑐ℎ𝑎𝑟𝑔𝑒+ 𝑈</a:t>
+                <a:t>𝑑𝑖𝑠𝑝𝑒𝑟𝑠𝑖𝑜𝑛+ </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>^</a:t>
+                <a:t>𝑉^</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="es-ES" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑑𝑖𝑠𝑝𝑒𝑟𝑠𝑖𝑜𝑛+ 𝑈</a:t>
+                <a:t>𝑟𝑒𝑝𝑢𝑙𝑠𝑖𝑜𝑛+ </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>^</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="es-ES" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑟𝑒𝑝𝑢𝑙𝑠𝑖𝑜𝑛+ 𝑈</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>^</a:t>
+                <a:t>𝑉^</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="es-ES" sz="1200" b="0" i="0">
@@ -4496,9 +4494,9 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>508000</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1303049" cy="490904"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="1332736" cy="490904"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -4512,8 +4510,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4578350" y="10820400"/>
-              <a:ext cx="1303049" cy="490904"/>
+              <a:off x="4582746" y="10362712"/>
+              <a:ext cx="1332736" cy="490904"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4557,10 +4555,10 @@
                       </m:sSupPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑈</m:t>
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑉</m:t>
                         </m:r>
                       </m:e>
                       <m:sup>
@@ -4711,7 +4709,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -4725,8 +4723,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4578350" y="10820400"/>
-              <a:ext cx="1303049" cy="490904"/>
+              <a:off x="4582746" y="10362712"/>
+              <a:ext cx="1332736" cy="490904"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4753,23 +4751,30 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑉^</a:t>
+              </a:r>
               <a:r>
                 <a:rPr lang="es-ES" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑈</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>^</a:t>
+                <a:t>𝑐ℎ𝑎𝑟𝑔𝑒= </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∑_(</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="es-ES" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑐ℎ𝑎𝑟𝑔𝑒= ∑8_(𝑖&lt;𝑗)▒(𝑞^𝑖 𝑞^𝑗)/𝑟^𝑖𝑗 </a:t>
+                <a:t>𝑖&lt;𝑗)▒(𝑞^𝑖 𝑞^𝑗)/𝑟^𝑖𝑗 </a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1200"/>
             </a:p>
@@ -4787,8 +4792,8 @@
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3559692" cy="503728"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -4847,10 +4852,10 @@
                       </m:sSupPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑈</m:t>
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑉</m:t>
                         </m:r>
                       </m:e>
                       <m:sup>
@@ -5315,7 +5320,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -5357,23 +5362,30 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑉^</a:t>
+              </a:r>
               <a:r>
                 <a:rPr lang="es-ES" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑈</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>^</a:t>
+                <a:t>𝑑𝑖𝑠𝑝𝑒𝑟𝑠𝑖𝑜𝑛=−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" altLang="zh-CN" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∑_(</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="es-ES" sz="1200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑑𝑖𝑠𝑝𝑒𝑟𝑠𝑖𝑜𝑛=−∑_(𝑖&lt;𝑗)▒〖(〖𝑓_6〗^𝑖𝑗 (𝑟^𝑖𝑗 )  〖𝐶_6〗^𝑖𝑗/(𝑟^𝑖𝑗 )^6 +〖𝑓_8〗^𝑖𝑗 (𝑟^𝑖𝑗 )  〖𝐶_8〗^𝑖𝑗/(𝑟^𝑖𝑗 )^8 〗  </a:t>
+                <a:t>𝑖&lt;𝑗)▒〖(〖𝑓_6〗^𝑖𝑗 (𝑟^𝑖𝑗 )  〖𝐶_6〗^𝑖𝑗/(𝑟^𝑖𝑗 )^6 +〖𝑓_8〗^𝑖𝑗 (𝑟^𝑖𝑗 )  〖𝐶_8〗^𝑖𝑗/(𝑟^𝑖𝑗 )^8 〗  </a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1200"/>
             </a:p>
@@ -5850,354 +5862,6 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>118534</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>922867</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="998350" cy="197875"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="15" name="TextBox 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AF6FBA4-307F-F74D-A6E2-72123E098916}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4580467" y="13512800"/>
-              <a:ext cx="998350" cy="197875"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSup>
-                      <m:sSupPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1200" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSupPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑈</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sup>
-                        <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑝𝑜𝑙𝑎𝑟𝑖𝑧𝑎𝑡𝑖𝑜𝑛</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>= </m:t>
-                        </m:r>
-                      </m:sup>
-                    </m:sSup>
-                    <m:r>
-                      <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t> </m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1200"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="15" name="TextBox 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AF6FBA4-307F-F74D-A6E2-72123E098916}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4580467" y="13512800"/>
-              <a:ext cx="998350" cy="197875"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="es-ES" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑈</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>^(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="es-ES" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑝𝑜𝑙𝑎𝑟𝑖𝑧𝑎𝑡𝑖𝑜𝑛= </a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="es-ES" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>  </a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1200"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>474134</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="882999" cy="197875"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="16" name="TextBox 15">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{404F4359-57D2-2849-8BDD-CEE66318E871}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4563533" y="13064067"/>
-              <a:ext cx="882999" cy="197875"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSup>
-                      <m:sSupPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1200" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSupPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑈</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sup>
-                        <m:r>
-                          <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑟𝑒𝑝𝑢𝑙𝑠𝑖𝑜𝑛</m:t>
-                        </m:r>
-                      </m:sup>
-                    </m:sSup>
-                    <m:r>
-                      <a:rPr lang="es-ES" sz="1200" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>= </m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1200"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="16" name="TextBox 15">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{404F4359-57D2-2849-8BDD-CEE66318E871}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4563533" y="13064067"/>
-              <a:ext cx="882999" cy="197875"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="es-ES" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑈</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>^</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="es-ES" sz="1200" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑟𝑒𝑝𝑢𝑙𝑠𝑖𝑜𝑛= </a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1200"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
       <xdr:colOff>4761</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
@@ -8047,16 +7711,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>1295400</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1666876</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>666750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>1434601</xdr:rowOff>
+      <xdr:rowOff>1570149</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8072,7 +7736,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -8085,8 +7749,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4552950" y="13401675"/>
-          <a:ext cx="5248275" cy="1472701"/>
+          <a:off x="1666876" y="14106525"/>
+          <a:ext cx="3219450" cy="903399"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8137,6 +7801,306 @@
         <a:xfrm>
           <a:off x="4391025" y="15916275"/>
           <a:ext cx="5248275" cy="516975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>266701</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2676526</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>248281</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="图片 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FDFFBA7-05B1-CF1C-5E97-9E85489660D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524376" y="12372976"/>
+          <a:ext cx="2609850" cy="1315080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2771775</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>652679</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="图片 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BE1F0C9-CF82-FF87-321A-13B319CB2BCB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7229475" y="12296775"/>
+          <a:ext cx="2324100" cy="462179"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2762251</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>704850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1133476</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1089875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="图片 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95402CA-3DA3-D912-1CF2-3C0199E306E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7219951" y="12811125"/>
+          <a:ext cx="3124200" cy="385025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>314326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2798043</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1724026</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="图片 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E4DC2E1-FB85-DCBD-9DFF-0CCBF0EBABBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4533900" y="13754101"/>
+          <a:ext cx="2721843" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2628901</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>295276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1381126</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>612268</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="图片 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E44E1EB-A714-D9B2-6429-A73DE9190FF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7086601" y="13735051"/>
+          <a:ext cx="3505200" cy="316992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2876550</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>666751</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>232739</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1752601</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="图片 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B26C5BC-D4F4-CD3A-6B84-3F2686BEEB3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7334250" y="14106526"/>
+          <a:ext cx="2109164" cy="1085850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8438,25 +8402,25 @@
   </sheetPr>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="62.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="62.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75" customHeight="1">
+    <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8483,83 +8447,83 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="23" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="30">
         <v>2</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="24"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="32"/>
       <c r="M3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="28.8">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="28" t="s">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="42" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="29"/>
+    <row r="5" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="31.2" customHeight="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="20"/>
+    <row r="6" spans="1:13" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="10" t="s">
         <v>19</v>
       </c>
@@ -8567,26 +8531,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="31.2" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="20"/>
+    <row r="7" spans="1:13" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="28.8">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="20"/>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="10" t="s">
         <v>22</v>
       </c>
@@ -8594,133 +8558,133 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="43.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="20"/>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="43.2">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="22"/>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="20"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="24"/>
+      <c r="I10" s="32"/>
     </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A11" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="19" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="30">
         <v>2</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="35" t="s">
+      <c r="H11" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="24"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="32"/>
     </row>
-    <row r="13" spans="1:13" ht="28.8">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="20"/>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="32"/>
     </row>
-    <row r="14" spans="1:13" ht="43.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="19" t="s">
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="20"/>
+      <c r="G14" s="27"/>
       <c r="H14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="24"/>
+      <c r="I14" s="32"/>
     </row>
-    <row r="15" spans="1:13" ht="43.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="20"/>
+    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="24"/>
+      <c r="I15" s="32"/>
     </row>
-    <row r="16" spans="1:13" ht="57.6">
-      <c r="A16" s="30" t="s">
+    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="45" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="30">
         <v>2</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="26" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="6" t="s">
@@ -8728,31 +8692,31 @@
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="43.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="22"/>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="20"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="6" t="s">
         <v>39</v>
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" ht="100.8">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="22"/>
+    <row r="18" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="31"/>
       <c r="F18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="20"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="5" t="s">
         <v>41</v>
       </c>
@@ -8760,40 +8724,40 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="78" customHeight="1">
-      <c r="A19" s="30" t="s">
+    <row r="19" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="45" t="s">
+      <c r="C19" s="26"/>
+      <c r="D19" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="30">
         <v>3</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="26" t="s">
         <v>29</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="96" customHeight="1">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="22"/>
+    <row r="20" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="20"/>
+      <c r="G20" s="27"/>
       <c r="H20" s="6" t="s">
         <v>47</v>
       </c>
@@ -8801,17 +8765,17 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="88.95" customHeight="1">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:9" ht="88.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="31" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="7">
@@ -8820,73 +8784,73 @@
       <c r="F21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="24"/>
-      <c r="I21" s="19" t="s">
+      <c r="H21" s="32"/>
+      <c r="I21" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="88.2" customHeight="1">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="22"/>
+    <row r="22" spans="1:9" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="7">
         <v>2</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="19"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="37"/>
     </row>
-    <row r="23" spans="1:9" ht="105" customHeight="1">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="22"/>
+    <row r="23" spans="1:9" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="7">
         <v>2</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="19"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="37"/>
     </row>
-    <row r="24" spans="1:9" ht="160.19999999999999" customHeight="1">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="22"/>
+    <row r="24" spans="1:9" ht="160.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="7">
         <v>3</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="19"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="37"/>
     </row>
-    <row r="25" spans="1:9" ht="60" customHeight="1">
-      <c r="A25" s="39" t="s">
+    <row r="25" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="25" t="s">
         <v>65</v>
       </c>
       <c r="D25" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="35" t="s">
         <v>63</v>
       </c>
       <c r="F25" s="6" t="s">
@@ -8902,12 +8866,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="67.95" customHeight="1">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
+    <row r="26" spans="1:9" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="32"/>
+      <c r="E26" s="36"/>
       <c r="F26" s="15" t="s">
         <v>61</v>
       </c>
@@ -8919,15 +8883,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="57.6">
-      <c r="A27" s="39" t="s">
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="42" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="22" t="s">
         <v>69</v>
       </c>
       <c r="E27" s="7">
@@ -8936,45 +8900,70 @@
       <c r="F27" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G27" s="39" t="s">
+      <c r="G27" s="19" t="s">
         <v>73</v>
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="72">
-      <c r="A28" s="41"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="43"/>
+    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="7">
         <v>2</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="41"/>
+      <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="28.8">
-      <c r="A29" s="38"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="44"/>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="24"/>
       <c r="E29" s="7">
         <v>3</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G29" s="38"/>
+      <c r="G29" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="G27:G29"/>
+    <mergeCell ref="I21:I24"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="G21:G24"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="E2:E10"/>
+    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="G2:G10"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H21:H24"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="A25:A26"/>
@@ -8991,36 +8980,11 @@
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="E16:E18"/>
     <mergeCell ref="G25:G26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G15"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H21:H24"/>
-    <mergeCell ref="I11:I15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="F2:F9"/>
-    <mergeCell ref="G2:G10"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="D2:D10"/>
-    <mergeCell ref="E2:E10"/>
-    <mergeCell ref="I21:I24"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="G21:G24"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="G27:G29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
test on lj energy min
</commit_message>
<xml_diff>
--- a/literature/review/potential_comparisons.xlsx
+++ b/literature/review/potential_comparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\School\FFparamOpt\literature\review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7012C9-D4C4-4E7B-856E-DCA003157943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD89D998-EBB0-49E1-977B-5C2431A9B407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -487,26 +487,68 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -520,53 +562,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1291,8 +1291,8 @@
       <xdr:rowOff>248920</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2419350" cy="558800"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1654,7 +1654,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -8438,8 +8438,8 @@
   </sheetPr>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -8484,55 +8484,55 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="23" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="30">
         <v>2</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="24"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="32"/>
       <c r="M3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="28.8">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="28" t="s">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="42" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -8540,26 +8540,26 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="29"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="31.2" customHeight="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="20"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="10" t="s">
         <v>19</v>
       </c>
@@ -8568,25 +8568,25 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="31.2" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="20"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="28.8">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="20"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="10" t="s">
         <v>22</v>
       </c>
@@ -8595,132 +8595,132 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="43.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="20"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="37" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="43.2">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="22"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="20"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="24"/>
+      <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="19" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="30">
         <v>2</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="35" t="s">
+      <c r="H11" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="37" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="24"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="32"/>
     </row>
     <row r="13" spans="1:13" ht="28.8">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="20"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:13" ht="43.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="19" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="20"/>
+      <c r="G14" s="27"/>
       <c r="H14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="24"/>
+      <c r="I14" s="32"/>
     </row>
     <row r="15" spans="1:13" ht="43.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="20"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="24"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:13" ht="57.6">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="45" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="30">
         <v>2</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="26" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="6" t="s">
@@ -8729,30 +8729,30 @@
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" ht="43.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="22"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="20"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="6" t="s">
         <v>39</v>
       </c>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" ht="100.8">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="22"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="31"/>
       <c r="F18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="20"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="5" t="s">
         <v>41</v>
       </c>
@@ -8761,23 +8761,23 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="78" customHeight="1">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="45" t="s">
+      <c r="C19" s="26"/>
+      <c r="D19" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="30">
         <v>3</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="26" t="s">
         <v>29</v>
       </c>
       <c r="I19" s="14" t="s">
@@ -8785,15 +8785,15 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="96" customHeight="1">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="22"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="20"/>
+      <c r="G20" s="27"/>
       <c r="H20" s="6" t="s">
         <v>47</v>
       </c>
@@ -8802,16 +8802,16 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="88.95" customHeight="1">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="31" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="7">
@@ -8820,73 +8820,73 @@
       <c r="F21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="24"/>
-      <c r="I21" s="19" t="s">
+      <c r="H21" s="32"/>
+      <c r="I21" s="37" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="88.2" customHeight="1">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="22"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="7">
         <v>2</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="19"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="37"/>
     </row>
     <row r="23" spans="1:9" ht="105" customHeight="1">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="22"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="7">
         <v>2</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="19"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="37"/>
     </row>
     <row r="24" spans="1:9" ht="160.19999999999999" customHeight="1">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="22"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="7">
         <v>3</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="19"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="37"/>
     </row>
     <row r="25" spans="1:9" ht="60" customHeight="1">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="25" t="s">
         <v>65</v>
       </c>
       <c r="D25" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="35" t="s">
         <v>63</v>
       </c>
       <c r="F25" s="6" t="s">
@@ -8903,11 +8903,11 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="67.95" customHeight="1">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="32"/>
+      <c r="E26" s="36"/>
       <c r="F26" s="15" t="s">
         <v>61</v>
       </c>
@@ -8920,14 +8920,14 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="57.6">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="42" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="22" t="s">
         <v>69</v>
       </c>
       <c r="E27" s="7">
@@ -8936,45 +8936,70 @@
       <c r="F27" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G27" s="39" t="s">
+      <c r="G27" s="19" t="s">
         <v>73</v>
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="72">
-      <c r="A28" s="41"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="43"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="7">
         <v>2</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="41"/>
+      <c r="G28" s="20"/>
     </row>
     <row r="29" spans="1:9" ht="28.8">
-      <c r="A29" s="38"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="44"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="24"/>
       <c r="E29" s="7">
         <v>3</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G29" s="38"/>
+      <c r="G29" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="G27:G29"/>
+    <mergeCell ref="I21:I24"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="G21:G24"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="E2:E10"/>
+    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="G2:G10"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H21:H24"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="A25:A26"/>
@@ -8991,36 +9016,11 @@
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="E16:E18"/>
     <mergeCell ref="G25:G26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G15"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H21:H24"/>
-    <mergeCell ref="I11:I15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="F2:F9"/>
-    <mergeCell ref="G2:G10"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="D2:D10"/>
-    <mergeCell ref="E2:E10"/>
-    <mergeCell ref="I21:I24"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="G21:G24"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="G27:G29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>